<commit_message>
Back to best solution with single thread.
</commit_message>
<xml_diff>
--- a/RouletteStrategy/RegressionAnalysis.xlsx
+++ b/RouletteStrategy/RegressionAnalysis.xlsx
@@ -24,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Looks like an exponential function</t>
   </si>
   <si>
     <t>Constant base, variable exponent</t>
+  </si>
+  <si>
+    <t>Roll</t>
   </si>
   <si>
     <t>Bet</t>
@@ -51,6 +54,54 @@
   </si>
   <si>
     <t>Grey line: ceiling of upper bound</t>
+  </si>
+  <si>
+    <t>Payout</t>
+  </si>
+  <si>
+    <t>Min Bet</t>
+  </si>
+  <si>
+    <t>Max Bet</t>
+  </si>
+  <si>
+    <t>Board Hits</t>
+  </si>
+  <si>
+    <t>*All with break evens allowed</t>
+  </si>
+  <si>
+    <t>The lower bound line should work like lower bound rolls</t>
+  </si>
+  <si>
+    <t>upper bound could be lower bound plus min bet times payout factor</t>
+  </si>
+  <si>
+    <t>Testing with 1 to 50 Columns:</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>1 to 20 with lines</t>
+  </si>
+  <si>
+    <t>y = (1/2) * (1 + (1/2)^x</t>
+  </si>
+  <si>
+    <t>y = (1/2) * (1 + (1/5)^x</t>
+  </si>
+  <si>
+    <t>Should be able to use this equation up until the stake where the roll is limited due to the max bet</t>
+  </si>
+  <si>
+    <t>Actually don't even need a lower bound because of the way the algorithm works, we just need an upper bound</t>
+  </si>
+  <si>
+    <t>Possible Upper Bound?</t>
+  </si>
+  <si>
+    <t>y = (1.5^x)</t>
   </si>
 </sst>
 </file>
@@ -74,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -82,12 +133,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -172,7 +236,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:f>Sheet1!$A$27:$A$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -241,7 +305,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$21</c:f>
+              <c:f>Sheet1!$B$27:$B$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -332,7 +396,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:f>Sheet1!$A$27:$A$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -401,7 +465,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$21</c:f>
+              <c:f>Sheet1!$C$27:$C$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -492,7 +556,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:f>Sheet1!$A$27:$A$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -561,7 +625,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$21</c:f>
+              <c:f>Sheet1!$D$27:$D$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -830,7 +894,1121 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$53:$A$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$53:$B$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7BA2-4957-9C09-9D6F456C56B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$53:$A$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$53:$C$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.53125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.796875</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.6953125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.54296875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.814453125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19.2216796875</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28.83251953125</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43.248779296875</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.8731689453125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7BA2-4957-9C09-9D6F456C56B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="599660896"/>
+        <c:axId val="599664176"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="599660896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="599664176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="599664176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="599660896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$67:$A$86</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$67:$B$86</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F673-4CA1-BB28-32AE879B4849}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$67:$A$86</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$67:$C$86</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.86399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0367999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2441599999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4929919999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7915903999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1499084799999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5798901759999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0958682111999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.7150418534399994</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.4580502241279989</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.349660268953599</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.4195923227443181</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.7035107872931823</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.2442129447518173</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11.093055533702181</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13.311666640442617</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15.973999968531141</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.168799962237369</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F673-4CA1-BB28-32AE879B4849}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="464678976"/>
+        <c:axId val="464679960"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="464678976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="464679960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="464679960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="464678976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1386,19 +2564,1051 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>409574</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>533399</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1419,6 +3629,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E7C9B4D-191C-4676-A9E6-BF514CDC3462}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9831328E-C630-4EC0-8CAF-5B6F74B644B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1724,365 +4006,1026 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="35.28515625" customWidth="1"/>
     <col min="4" max="4" width="33.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <f>(0.5345405936)*(1.190684898^A2) - 1</f>
-        <v>-0.36353058783252457</v>
-      </c>
-      <c r="D2">
-        <f>(0.5345405936)*(1.190684898^A2) + 8</f>
-        <v>8.6364694121674752</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C21" si="0">(0.5345405936)*(1.190684898^A3) - 1</f>
-        <v>-0.24216548289324957</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D21" si="1">(0.5345405936)*(1.190684898^A3) + 8</f>
-        <v>8.7578345171067511</v>
-      </c>
-      <c r="N3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>-9.7657885297869673E-2</v>
+        <f>(1/2)*(1.5^A4)</f>
+        <v>0.75</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
-        <v>8.9023421147021295</v>
-      </c>
-      <c r="N4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <f>1.5^A4</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>7.4405128805210552E-2</v>
+        <f t="shared" ref="C5:C15" si="0">(1/2)*(1.5^A5)</f>
+        <v>1.125</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
-        <v>9.0744051288052106</v>
-      </c>
-      <c r="N5" t="s">
+        <f t="shared" ref="D5:D15" si="1">1.5^A5</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>0.27927796120210902</v>
+        <v>1.6875</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>9.2792779612021086</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3.375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0.52321694874758107</v>
+        <v>2.53125</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>9.5232169487475815</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5.0625</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>0.81367141725138459</v>
+        <v>3.796875</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>9.8136714172513848</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>7.59375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>1.1595111664554807</v>
+        <v>5.6953125</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>10.159511166455481</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>11.390625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>1.571297332960905</v>
+        <v>8.54296875</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>10.571297332960905</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>17.0859375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>2.0616049026242269</v>
+        <v>12.814453125</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>11.061604902624227</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>25.62890625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>2.6454067211974279</v>
+        <v>19.2216796875</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>11.645406721197428</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>38.443359375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>3.3405307299974742</v>
+        <v>28.83251953125</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>12.340530729997475</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>5</v>
+        <v>57.6650390625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1">
+        <v>38</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>4.1682043895129084</v>
+        <v>43.248779296875</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>13.168204389512908</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>86.49755859375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>5.153702916370329</v>
+        <v>64.8731689453125</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
+        <v>129.746337890625</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <f>(0.5345405936)*(1.190684898^A27) - 1</f>
+        <v>-0.36353058783252457</v>
+      </c>
+      <c r="D27">
+        <f>(0.5345405936)*(1.190684898^A27) + 8</f>
+        <v>8.6364694121674752</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ref="C28:C46" si="2">(0.5345405936)*(1.190684898^A28) - 1</f>
+        <v>-0.24216548289324957</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ref="D28:D46" si="3">(0.5345405936)*(1.190684898^A28) + 8</f>
+        <v>8.7578345171067511</v>
+      </c>
+      <c r="N28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>-9.7657885297869673E-2</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="3"/>
+        <v>8.9023421147021295</v>
+      </c>
+      <c r="N29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>7.4405128805210552E-2</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="3"/>
+        <v>9.0744051288052106</v>
+      </c>
+      <c r="N30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>0.27927796120210902</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="3"/>
+        <v>9.2792779612021086</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>0.52321694874758107</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="3"/>
+        <v>9.5232169487475815</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>7</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>0.81367141725138459</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="3"/>
+        <v>9.8136714172513848</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>8</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>1.1595111664554807</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="3"/>
+        <v>10.159511166455481</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>9</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>1.571297332960905</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="3"/>
+        <v>10.571297332960905</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>10</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>2.0616049026242269</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="3"/>
+        <v>11.061604902624227</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>11</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>2.6454067211974279</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="3"/>
+        <v>11.645406721197428</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>12</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>3.3405307299974742</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="3"/>
+        <v>12.340530729997475</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>13</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="2"/>
+        <v>4.1682043895129084</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="3"/>
+        <v>13.168204389512908</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>14</v>
+      </c>
+      <c r="B40">
+        <v>6</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="2"/>
+        <v>5.153702916370329</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="3"/>
         <v>14.153702916370328</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B41">
         <v>7</v>
       </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
+      <c r="C41">
+        <f t="shared" si="2"/>
         <v>6.3271211293007079</v>
       </c>
-      <c r="D16">
-        <f t="shared" si="1"/>
+      <c r="D41">
+        <f t="shared" si="3"/>
         <v>15.327121129300707</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B42">
         <v>8</v>
       </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
+      <c r="C42">
+        <f t="shared" si="2"/>
         <v>7.7242924744750585</v>
       </c>
-      <c r="D17">
-        <f t="shared" si="1"/>
+      <c r="D42">
+        <f t="shared" si="3"/>
         <v>16.724292474475057</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B43">
         <v>12</v>
       </c>
-      <c r="C18">
-        <f t="shared" si="0"/>
+      <c r="C43">
+        <f t="shared" si="2"/>
         <v>9.3878832950925037</v>
       </c>
-      <c r="D18">
-        <f t="shared" si="1"/>
+      <c r="D43">
+        <f t="shared" si="3"/>
         <v>18.387883295092504</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>18</v>
+      </c>
+      <c r="B44">
+        <v>20</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="2"/>
+        <v>11.368695761653122</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="3"/>
+        <v>20.368695761653122</v>
+      </c>
+      <c r="F44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>19</v>
+      </c>
+      <c r="B45">
+        <v>20</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="2"/>
+        <v>13.727219251356978</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="3"/>
+        <v>22.727219251356978</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>20</v>
+      </c>
+      <c r="B46">
+        <v>20</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="2"/>
+        <v>16.53547755212562</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="3"/>
+        <v>25.53547755212562</v>
+      </c>
+      <c r="F46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" t="s">
+        <v>10</v>
+      </c>
+      <c r="I47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <f>(1/2)*(1.5^A53)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <f t="shared" ref="C54:C64" si="4">(1/2)*(1.5^A54)</f>
+        <v>1.125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>3</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="4"/>
+        <v>1.6875</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>4</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="4"/>
+        <v>2.53125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>5</v>
+      </c>
+      <c r="B57">
+        <v>3</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="4"/>
+        <v>3.796875</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>6</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="4"/>
+        <v>5.6953125</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="B59">
+        <v>6</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="4"/>
+        <v>8.54296875</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>8</v>
+      </c>
+      <c r="B60">
+        <v>9</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="4"/>
+        <v>12.814453125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>9</v>
+      </c>
+      <c r="B61">
+        <v>14</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="4"/>
+        <v>19.2216796875</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>10</v>
+      </c>
+      <c r="B62">
+        <v>21</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="4"/>
+        <v>28.83251953125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>11</v>
+      </c>
+      <c r="B63" s="1">
+        <v>38</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="4"/>
+        <v>43.248779296875</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>12</v>
+      </c>
+      <c r="B64">
+        <v>50</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="4"/>
+        <v>64.8731689453125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <f>(1/2)*(1.2^A67)</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <f t="shared" ref="C68:C86" si="5">(1/2)*(1.2^A68)</f>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>3</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="5"/>
+        <v>0.86399999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>4</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="5"/>
+        <v>1.0367999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>5</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="5"/>
+        <v>1.2441599999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>6</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="5"/>
+        <v>1.4929919999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>7</v>
+      </c>
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="5"/>
+        <v>1.7915903999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>8</v>
+      </c>
+      <c r="B74">
+        <v>2</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="5"/>
+        <v>2.1499084799999997</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>9</v>
+      </c>
+      <c r="B75">
+        <v>2</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="5"/>
+        <v>2.5798901759999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>10</v>
+      </c>
+      <c r="B76">
+        <v>3</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="5"/>
+        <v>3.0958682111999996</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>11</v>
+      </c>
+      <c r="B77">
+        <v>3</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="5"/>
+        <v>3.7150418534399994</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>12</v>
+      </c>
+      <c r="B78">
+        <v>4</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="5"/>
+        <v>4.4580502241279989</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>13</v>
+      </c>
+      <c r="B79">
+        <v>5</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="5"/>
+        <v>5.349660268953599</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>14</v>
+      </c>
+      <c r="B80">
+        <v>6</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="5"/>
+        <v>6.4195923227443181</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>15</v>
+      </c>
+      <c r="B81">
+        <v>7</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="5"/>
+        <v>7.7035107872931823</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>16</v>
+      </c>
+      <c r="B82">
+        <v>8</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="5"/>
+        <v>9.2442129447518173</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>17</v>
+      </c>
+      <c r="B83" s="1">
+        <v>12</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="5"/>
+        <v>11.093055533702181</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B84">
         <v>20</v>
       </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>11.368695761653122</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="1"/>
-        <v>20.368695761653122</v>
-      </c>
-      <c r="F19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="C84">
+        <f t="shared" si="5"/>
+        <v>13.311666640442617</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B85">
         <v>20</v>
       </c>
-      <c r="C20">
-        <f t="shared" si="0"/>
-        <v>13.727219251356978</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="1"/>
-        <v>22.727219251356978</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="C85">
+        <f t="shared" si="5"/>
+        <v>15.973999968531141</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B86">
         <v>20</v>
       </c>
-      <c r="C21">
-        <f t="shared" si="0"/>
-        <v>16.53547755212562</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="1"/>
-        <v>25.53547755212562</v>
+      <c r="C86">
+        <f t="shared" si="5"/>
+        <v>19.168799962237369</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="C87" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First single threaded solution that seems to be workign with upper bound.
</commit_message>
<xml_diff>
--- a/RouletteStrategy/RegressionAnalysis.xlsx
+++ b/RouletteStrategy/RegressionAnalysis.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
   <si>
     <t>Looks like an exponential function</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>y =(1 + (1/1))^x</t>
+  </si>
+  <si>
+    <t>1 to 25 Corners</t>
   </si>
 </sst>
 </file>
@@ -14751,10 +14754,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A138" sqref="A138"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H135" sqref="H135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17113,6 +17116,31 @@
         <v>20</v>
       </c>
     </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>2</v>
+      </c>
+      <c r="B140" t="s">
+        <v>18</v>
+      </c>
+      <c r="C140" t="s">
+        <v>36</v>
+      </c>
+      <c r="D140" t="s">
+        <v>26</v>
+      </c>
+      <c r="E140" t="s">
+        <v>25</v>
+      </c>
+      <c r="F140" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>